<commit_message>
los 3 requerimientos de cambio de cambios estan cumplidos y testeados como lic# ifta# tex/ein# ok
</commit_message>
<xml_diff>
--- a/requerimientos-Trucks.xlsx
+++ b/requerimientos-Trucks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t xml:space="preserve">Tareas</t>
   </si>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">tax id # ein varchar </t>
   </si>
   <si>
-    <t xml:space="preserve">lic </t>
+    <t xml:space="preserve">numero_lic_emp varchar</t>
   </si>
   <si>
     <t xml:space="preserve">boton que lleve a pagina donde muestre tabla alcohol y drogas y este filtrado por esos dos servicios y ademas se deben enviar un emaill por medio de un boton  que seleccione 25% de los clientes filtarados ya por esos dos servicios</t>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -168,6 +168,22 @@
       <color rgb="FF843C0B"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -242,7 +258,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,6 +309,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -373,19 +405,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E37"/>
+  <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="88.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.05"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -393,15 +425,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -409,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -417,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -425,7 +457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -434,7 +466,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -443,7 +475,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
@@ -451,24 +483,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
@@ -476,7 +508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
@@ -484,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
@@ -492,7 +524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
@@ -500,80 +532,110 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4"/>
       <c r="C19" s="12"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4"/>
       <c r="C20" s="12"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="C28" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="C10:C14"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
completamos 2 requerimientos mas debes revisar el excel de requerimientos para mas detalles
</commit_message>
<xml_diff>
--- a/requerimientos-Trucks.xlsx
+++ b/requerimientos-Trucks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos_BD\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09DE96-0108-44EB-B61E-EEFF43F6A1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9605C213-6661-462D-A9F5-37DD82544B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Tareas</t>
   </si>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -173,6 +173,18 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -231,23 +243,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,6 +271,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -657,146 +676,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E38"/>
+  <dimension ref="B2:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="88.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="11"/>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="12"/>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="2:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -804,7 +823,7 @@
       <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -812,24 +831,27 @@
       <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="C24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="20"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="15"/>
+      <c r="C26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -837,48 +859,54 @@
       <c r="B28" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="19"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="19"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="1"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="19"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
modelamos los requerimientos en una  tabla dinamica
</commit_message>
<xml_diff>
--- a/requerimientos-Trucks.xlsx
+++ b/requerimientos-Trucks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos_BD\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9605C213-6661-462D-A9F5-37DD82544B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E92768-90F1-4E43-A547-E1FF64D5109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dinamica-RQ" sheetId="2" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
   <si>
     <t>Tareas</t>
   </si>
@@ -112,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -123,14 +124,6 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF843C0B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -149,23 +142,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF843C0B"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
@@ -184,12 +163,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,18 +190,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEDEDED"/>
+        <fgColor theme="0"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -238,67 +248,437 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF525252"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -377,6 +757,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F335F52-4723-4886-8669-A761397ED4A5}" name="Tabla3" displayName="Tabla3" ref="B2:C24" totalsRowShown="0" tableBorderDxfId="9">
+  <autoFilter ref="B2:C24" xr:uid="{4F335F52-4723-4886-8669-A761397ED4A5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C24">
+    <sortCondition sortBy="cellColor" ref="B2:B24" dxfId="6"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{865B3DDD-E1B0-454E-B147-7119534E8AFA}" name="Tareas" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{49508478-4791-4B40-8CB3-CDB53002679A}" name="Estado" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,11 +1069,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBF2930-735F-4BF1-B2A2-D6A777D17877}">
+  <dimension ref="B1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="91.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E43"/>
+  <dimension ref="B1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="B1:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,234 +1295,227 @@
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>1</v>
-      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="2:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="C8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="2:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>6</v>
-      </c>
+      <c r="C9" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
+      <c r="C10" s="30"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>6</v>
+      <c r="B18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="B23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="23"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="20"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="10"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="25"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="19"/>
+      <c r="B28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="14"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="19"/>
+      <c r="B30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="14"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="16"/>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="12" t="s">
+      <c r="B31" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="17"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
   </mergeCells>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se cumlen la mayoria de los requerimientos y se esperan instrucciones
</commit_message>
<xml_diff>
--- a/requerimientos-Trucks.xlsx
+++ b/requerimientos-Trucks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos_BD\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E92768-90F1-4E43-A547-E1FF64D5109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E7657D-A966-4AAE-901E-145837D3A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
   <si>
     <t>Tareas</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>mostrar perfil y rol en la info del perfil al lado de la foto</t>
+  </si>
+  <si>
+    <t>Medianamente listo</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +227,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -378,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,107 +447,117 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -532,7 +569,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF525252"/>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -540,7 +577,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF525252"/>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -548,7 +585,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF525252"/>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -556,7 +593,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF525252"/>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -564,7 +601,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF525252"/>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -572,7 +609,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF525252"/>
-          <bgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -763,7 +800,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F335F52-4723-4886-8669-A761397ED4A5}" name="Tabla3" displayName="Tabla3" ref="B2:C24" totalsRowShown="0" tableBorderDxfId="9">
   <autoFilter ref="B2:C24" xr:uid="{4F335F52-4723-4886-8669-A761397ED4A5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C24">
-    <sortCondition sortBy="cellColor" ref="B2:B24" dxfId="6"/>
+    <sortCondition sortBy="cellColor" ref="C2:C24" dxfId="1"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{865B3DDD-E1B0-454E-B147-7119534E8AFA}" name="Tareas" dataDxfId="8"/>
@@ -1073,112 +1110,116 @@
   <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C4" activeCellId="1" sqref="C5 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="91.42578125" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="51"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="51"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C10" s="46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+    <row r="11" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C11" s="45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C12" s="45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="45" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1186,7 +1227,7 @@
       <c r="B14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1194,7 +1235,7 @@
       <c r="B15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1202,31 +1243,31 @@
       <c r="B16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1234,7 +1275,7 @@
       <c r="B20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1242,7 +1283,7 @@
       <c r="B21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1250,7 +1291,7 @@
       <c r="B22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1258,22 +1299,23 @@
       <c r="B23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="26" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1296,16 +1338,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="37"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
@@ -1354,29 +1396,29 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
-      <c r="C10" s="30"/>
+      <c r="C10" s="35"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
-      <c r="C11" s="30"/>
+      <c r="C11" s="35"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
-      <c r="C12" s="30"/>
+      <c r="C12" s="35"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="36"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
@@ -1460,18 +1502,18 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="39"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="40"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
-      <c r="C26" s="25"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="41"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">

</xml_diff>